<commit_message>
uwb, tank, actuator sended to factory
</commit_message>
<xml_diff>
--- a/Linear Actuator V3.1/Project Outputs for Linear Actuator V3.1/BOM/Bill of Materials-Linear Actuator V3.1_BomDoc.xlsx
+++ b/Linear Actuator V3.1/Project Outputs for Linear Actuator V3.1/BOM/Bill of Materials-Linear Actuator V3.1_BomDoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\UAV-CAN-MODULES\Linear Actuator V3.1\Project Outputs for Linear Actuator V3.1\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\altium workspace\UAV-CAN-MODULES\Linear Actuator V3.1\Project Outputs for Linear Actuator V3.1\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F77AE80A-2A48-4C7A-963C-1BDA1B4A6B1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C0643C6-7FD7-4F94-835E-D5AB439F5385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6825" xr2:uid="{4A78D720-244E-449C-AD02-F17D5512FAE5}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{DEF96BE1-7D5B-488C-8C77-7ACC2993B8FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Linear Actuat" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,13 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -511,6 +518,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -563,7 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -579,9 +587,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -619,7 +627,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -725,7 +733,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -874,7 +882,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535DBF92-2CAE-49B8-A004-89562CA62640}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869A0FE5-6010-4A6C-B19F-614901B05DEF}">
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1791,6 +1799,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>